<commit_message>
added code about data matrix to table
</commit_message>
<xml_diff>
--- a/images/Other_Files/TblAsValues.xlsx
+++ b/images/Other_Files/TblAsValues.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Cloned_Repositories\Posts\images\Other_Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72BABD52-2565-4C2A-919B-8CA8B4990DBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{272C807E-270A-43D4-A4B9-A3C92219BCC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="96" yWindow="1920" windowWidth="22944" windowHeight="10164" activeTab="1" xr2:uid="{BBBA58B9-7304-4CDA-A74E-05451C99E376}"/>
+    <workbookView xWindow="96" yWindow="1920" windowWidth="22944" windowHeight="8052" activeTab="2" xr2:uid="{BBBA58B9-7304-4CDA-A74E-05451C99E376}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Arb_Tbl" sheetId="2" r:id="rId2"/>
+    <sheet name="Skills_Matrix" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="47">
   <si>
     <t>myHead1</t>
   </si>
@@ -147,6 +148,36 @@
   </si>
   <si>
     <t>Darryl</t>
+  </si>
+  <si>
+    <t>Alfred</t>
+  </si>
+  <si>
+    <t>Chris</t>
+  </si>
+  <si>
+    <t>Dante</t>
+  </si>
+  <si>
+    <t>Edgar</t>
+  </si>
+  <si>
+    <t>Brew</t>
+  </si>
+  <si>
+    <t>Filter</t>
+  </si>
+  <si>
+    <t>Pack</t>
+  </si>
+  <si>
+    <t>Ship</t>
+  </si>
+  <si>
+    <t>Manage</t>
+  </si>
+  <si>
+    <t>Column1</t>
   </si>
 </sst>
 </file>
@@ -249,6 +280,21 @@
     <tableColumn id="6" xr3:uid="{D35E76F1-0FA6-42A0-80B3-8AC4B75BCA04}" name="Hours"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{1164F606-9CD0-4986-A1C4-315B3883FFA4}" name="Skills_Mtx" displayName="Skills_Mtx" ref="A1:F6" totalsRowShown="0">
+  <autoFilter ref="A1:F6" xr:uid="{1164F606-9CD0-4986-A1C4-315B3883FFA4}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{ADBB0A26-DC95-487A-BA32-F4C63AA28114}" name="Column1"/>
+    <tableColumn id="2" xr3:uid="{EC6C7E3E-B054-462E-A7A4-3CD68F0EE88B}" name="Brew"/>
+    <tableColumn id="3" xr3:uid="{48A2B9B1-F9BE-45E9-8F7F-0D12EF1419A8}" name="Filter"/>
+    <tableColumn id="4" xr3:uid="{1DEC1F3D-C122-4D18-B493-1B49427CD779}" name="Pack"/>
+    <tableColumn id="5" xr3:uid="{A599B646-A59C-47B2-8BEA-71EC7E256E3B}" name="Ship"/>
+    <tableColumn id="6" xr3:uid="{D40C1AD0-CDEF-45EA-B0BE-373A867D1F6B}" name="Manage"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -739,7 +785,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E898CF44-CB42-49BE-BB13-B57007476583}">
   <dimension ref="A3:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
@@ -923,4 +969,146 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66E0A24E-69CD-4543-8D3C-5BB5A0B4B44B}">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.109375" customWidth="1"/>
+    <col min="6" max="6" width="9.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>